<commit_message>
last changes for tonight.
</commit_message>
<xml_diff>
--- a/MAS Spec.xlsx
+++ b/MAS Spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project holder\MAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B604E5BB-4E4B-4C3D-804C-7D426C2FDF9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B93556B-1A03-41B1-8291-EFF313BE8D01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18120" yWindow="-12930" windowWidth="18240" windowHeight="29040" firstSheet="5" activeTab="9" xr2:uid="{A5A08AE7-B814-4604-A72D-A6C54990E20D}"/>
+    <workbookView xWindow="-18120" yWindow="-12930" windowWidth="18240" windowHeight="29040" firstSheet="2" activeTab="11" xr2:uid="{A5A08AE7-B814-4604-A72D-A6C54990E20D}"/>
   </bookViews>
   <sheets>
     <sheet name="MAS" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,11 @@
     <sheet name="Blueprint" sheetId="10" r:id="rId5"/>
     <sheet name="Source" sheetId="11" r:id="rId6"/>
     <sheet name="U" sheetId="4" r:id="rId7"/>
-    <sheet name="CL0" sheetId="2" r:id="rId8"/>
-    <sheet name="CL1" sheetId="3" r:id="rId9"/>
-    <sheet name="CL2" sheetId="5" r:id="rId10"/>
-    <sheet name="CL3" sheetId="6" r:id="rId11"/>
-    <sheet name="CL4" sheetId="13" r:id="rId12"/>
+    <sheet name="L0" sheetId="2" r:id="rId8"/>
+    <sheet name="L1" sheetId="3" r:id="rId9"/>
+    <sheet name="L2" sheetId="5" r:id="rId10"/>
+    <sheet name="L3" sheetId="6" r:id="rId11"/>
+    <sheet name="L4" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="338">
   <si>
     <t>A dynamic, highly adaptable, programming language. (Currently only a concept)</t>
   </si>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>Unissembly</t>
-  </si>
-  <si>
-    <t>Unissembly - Universal Assembler (Imperative). A universal assembly language intended to be human comprehendable and easy on the eyes. Has different levels for abstraction support. (Ranging from 1:1 statement execution to multi-statement abstraction, statements are explicitly sub-categorized by their level of abstraction from direct opcodes) (Must have at least one IR-Framework or Assembler installed for a compatible Alias Set) (Essentially acts a writtable intermediary, pure data types only)</t>
   </si>
   <si>
     <t xml:space="preserve">Compiler </t>
@@ -1090,9 +1087,6 @@
     <t>Provides the owning scope of a symbol associated with a heap allocation.</t>
   </si>
   <si>
-    <t>Has some C++ like features when it comes to level of complexity associated with classes and template concepts</t>
-  </si>
-  <si>
     <t>scope.caller</t>
   </si>
   <si>
@@ -1100,6 +1094,35 @@
   </si>
   <si>
     <t>Used inconjunction with symbol.owner to do assignment of ownership across callstack.</t>
+  </si>
+  <si>
+    <t>Has some C++ like features when it comes to level of features available.</t>
+  </si>
+  <si>
+    <t>Has some functional like features when it comes to level of features available.</t>
+  </si>
+  <si>
+    <t>Unissembly - Universal Assembler (Imperative/Procedural). A universal assembly language intended to be human comprehendable and easy on the eyes. Has different levels for abstraction support. (Ranging from 1:1 statement execution to multi-statement abstraction, statements are explicitly sub-categorized by their level of abstraction from direct opcodes) (Must have at least one IR-Framework or Assembler installed for a compatible Alias Set) (Essentially acts a writtable intermediary, pure data types only)</t>
+  </si>
+  <si>
+    <t>MAS</t>
+  </si>
+  <si>
+    <t>MAS Language:
+The langauge used by the compiler and interpreter is defined in layers from 0 to 4 (so far). These layers are oriented by abstraction level / overhead provided by each layer. The layer to extent represents a different parasignm/s for programming which each have their own use cases.
+Unissembly is intended to be the "inline assembler" for the language.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intended layer usage:
+Layer 0 : Boostrapping the langauge.
+Layer 1 : Low-level drivers/kernels, and compiler / interpreter backends
+Layer 2 : C/C++, rust like langauge. (But not the more advanced features, keeps it basic)
+Layer 3 : C/C++, rust like langague. (Higher level of features / library available)
+Layer 4 : Functional paradignm language (F#, Haskell). </t>
+  </si>
+  <si>
+    <t>There is no data declaration or direct object state manipulation.
+Use layer 3 or below for that.</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1359,6 +1382,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2965,7 +2991,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3015,54 +3041,54 @@
     </row>
     <row r="8" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="32"/>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>33</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3070,10 +3096,10 @@
     </row>
     <row r="16" spans="1:2" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3140,7 +3166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601C789F-A70D-44BB-BC27-A6660557AFE0}">
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
@@ -3154,24 +3180,24 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
@@ -3185,7 +3211,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -3211,7 +3237,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
@@ -3225,7 +3251,7 @@
     </row>
     <row r="10" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B10" s="37"/>
       <c r="C10" s="37"/>
@@ -3244,7 +3270,7 @@
     </row>
     <row r="11" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -3275,7 +3301,7 @@
     </row>
     <row r="13" spans="1:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
@@ -3289,13 +3315,13 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="29"/>
       <c r="E14" s="29"/>
@@ -3317,13 +3343,13 @@
     </row>
     <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3348,18 +3374,18 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B22" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="C22" s="20" t="s">
         <v>187</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B23" s="46"/>
       <c r="C23" s="46"/>
@@ -3381,14 +3407,14 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B27" s="46"/>
       <c r="C27" s="46"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B28" s="46"/>
       <c r="C28" s="46"/>
@@ -3405,7 +3431,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B31" s="46"/>
       <c r="C31" s="46"/>
@@ -3422,20 +3448,20 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" s="47"/>
       <c r="C34" s="47"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -3455,46 +3481,46 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="C41" s="21" t="s">
         <v>330</v>
-      </c>
-      <c r="B41" s="21" t="s">
-        <v>331</v>
-      </c>
-      <c r="C41" s="21" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3509,13 +3535,13 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -3545,90 +3571,90 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="B52" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="B52" s="44" t="s">
-        <v>192</v>
-      </c>
       <c r="C52" s="44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B53" s="19"/>
       <c r="C53" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B54" s="19"/>
       <c r="C54" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B55" s="19"/>
       <c r="C55" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B56" s="19"/>
       <c r="C56" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="B57" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="B57" s="22" t="s">
-        <v>238</v>
-      </c>
       <c r="C57" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B59" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="C59" s="21" t="s">
         <v>240</v>
-      </c>
-      <c r="C59" s="21" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="21" t="s">
+        <v>311</v>
+      </c>
+      <c r="B60" s="21" t="s">
         <v>312</v>
-      </c>
-      <c r="B60" s="21" t="s">
-        <v>313</v>
       </c>
       <c r="C60" s="21"/>
     </row>
@@ -3639,7 +3665,7 @@
     </row>
     <row r="62" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="49" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B62" s="49"/>
       <c r="C62" s="49"/>
@@ -3672,7 +3698,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D25EFA-8543-4173-8538-C9C6D311089E}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:L4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3681,17 +3709,17 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="18" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B4" s="37"/>
       <c r="C4" s="37"/>
@@ -3715,26 +3743,62 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF95F533-B3C5-4574-91F1-62FB50CEC440}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>259</v>
-      </c>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+    </row>
+    <row r="6" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
+        <v>337</v>
+      </c>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="29"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A6:I6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3743,7 +3807,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54BB39E1-BBDA-433B-A2A0-5DB3473C70E3}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:B30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3757,7 +3823,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="11"/>
     </row>
@@ -3766,7 +3832,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="11"/>
     </row>
@@ -3793,25 +3859,25 @@
         <v>12</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>13</v>
+        <v>333</v>
       </c>
       <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>15</v>
       </c>
       <c r="C6" s="11"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>17</v>
       </c>
       <c r="C7" s="11"/>
     </row>
@@ -3827,21 +3893,21 @@
     </row>
     <row r="10" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="11"/>
       <c r="C10" s="11"/>
     </row>
     <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="36"/>
       <c r="C11" s="11"/>
     </row>
     <row r="12" spans="1:3" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="36"/>
       <c r="C12" s="11"/>
@@ -3851,14 +3917,18 @@
       <c r="B13" s="14"/>
       <c r="C13" s="11"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
+    <row r="14" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="50" t="s">
+        <v>335</v>
+      </c>
+      <c r="B14" s="50"/>
       <c r="C14" s="11"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
+    <row r="15" spans="1:3" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="50" t="s">
+        <v>336</v>
+      </c>
+      <c r="B15" s="50"/>
       <c r="C15" s="11"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -3925,9 +3995,11 @@
       <c r="B29" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3938,7 +4010,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6639ACC-0A68-4AD4-B81D-51ABE7ED177F}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3948,12 +4022,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3965,7 +4039,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF91EC3-9B9C-4C79-892E-9DBBC47CA9BC}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3975,102 +4051,102 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -4083,7 +4159,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA7B1279-2DF6-45E8-94EF-FF370892003B}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4094,7 +4172,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" s="15"/>
     </row>
@@ -4104,7 +4182,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="4"/>
     </row>
@@ -4114,34 +4192,34 @@
     </row>
     <row r="5" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4150,18 +4228,18 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="4"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -4182,22 +4260,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -4209,7 +4287,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82BA0CDD-8C14-436D-A306-11FCD102CD5F}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4224,7 +4304,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -4237,7 +4317,7 @@
   <dimension ref="A1:M96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+      <selection activeCell="A7" sqref="A7:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4250,17 +4330,17 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>79</v>
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
@@ -4292,7 +4372,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
@@ -4309,7 +4389,7 @@
     </row>
     <row r="7" spans="1:13" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -4326,7 +4406,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
@@ -4343,7 +4423,7 @@
     </row>
     <row r="9" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -4360,7 +4440,7 @@
     </row>
     <row r="10" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B10" s="37"/>
       <c r="C10" s="37"/>
@@ -4377,7 +4457,7 @@
     </row>
     <row r="11" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -4394,7 +4474,7 @@
     </row>
     <row r="12" spans="1:13" ht="222.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B12" s="37"/>
       <c r="C12" s="37"/>
@@ -4425,13 +4505,13 @@
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="43"/>
       <c r="E14" s="43"/>
@@ -4445,13 +4525,13 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" s="43"/>
       <c r="E15" s="43"/>
@@ -4465,13 +4545,13 @@
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="19" t="s">
         <v>95</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>96</v>
       </c>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
@@ -4485,13 +4565,13 @@
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D17" s="43"/>
       <c r="E17" s="43"/>
@@ -4505,13 +4585,13 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D18" s="43"/>
       <c r="E18" s="43"/>
@@ -4525,207 +4605,207 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>103</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="B24" s="22" t="s">
         <v>223</v>
       </c>
-      <c r="B24" s="22" t="s">
-        <v>224</v>
-      </c>
       <c r="C24" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="C25" s="21" t="s">
         <v>158</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
     </row>
     <row r="27" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A27" s="45" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B27" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C27" s="45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>98</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>234</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="B29" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="C29" s="20" t="s">
         <v>216</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
+        <v>241</v>
+      </c>
+      <c r="B30" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="C30" s="21" t="s">
         <v>243</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="B33" s="20" t="s">
-        <v>107</v>
-      </c>
       <c r="C33" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="C34" s="20" t="s">
         <v>146</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" s="20" t="s">
         <v>155</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="C37" s="20" t="s">
         <v>153</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="C37" s="20" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -4735,144 +4815,144 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B39" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" s="20" t="s">
         <v>187</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B40" s="46"/>
       <c r="C40" s="46"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B41" s="20"/>
       <c r="C41" s="20"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B42" s="20"/>
       <c r="C42" s="20"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B43" s="20"/>
       <c r="C43" s="20"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B44" s="20"/>
       <c r="C44" s="20"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B45" s="20"/>
       <c r="C45" s="20"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B46" s="20"/>
       <c r="C46" s="20"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B47" s="20"/>
       <c r="C47" s="20"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B48" s="46"/>
       <c r="C48" s="46"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B49" s="46"/>
       <c r="C49" s="46"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B50" s="20"/>
       <c r="C50" s="20"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B52" s="20"/>
       <c r="C52" s="20"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B53" s="20"/>
       <c r="C53" s="20"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B55" s="20"/>
       <c r="C55" s="20"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B56" s="46"/>
       <c r="C56" s="46"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B57" s="20"/>
       <c r="C57" s="20"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B58" s="20"/>
       <c r="C58" s="20"/>
@@ -4884,204 +4964,204 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B60" s="23"/>
       <c r="C60" s="23"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B62" s="20" t="s">
         <v>121</v>
-      </c>
-      <c r="B62" s="20" t="s">
-        <v>122</v>
       </c>
       <c r="C62" s="20"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C63" s="20"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C64" s="20"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C65" s="20"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C67" s="20"/>
     </row>
     <row r="68" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C68" s="20"/>
     </row>
     <row r="69" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="B69" s="20" t="s">
         <v>133</v>
-      </c>
-      <c r="B69" s="20" t="s">
-        <v>134</v>
       </c>
       <c r="C69" s="20"/>
     </row>
     <row r="70" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B70" s="20" t="s">
         <v>135</v>
-      </c>
-      <c r="B70" s="20" t="s">
-        <v>136</v>
       </c>
       <c r="C70" s="20"/>
     </row>
     <row r="71" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="B71" s="20" t="s">
         <v>137</v>
-      </c>
-      <c r="B71" s="20" t="s">
-        <v>138</v>
       </c>
       <c r="C71" s="20"/>
     </row>
     <row r="72" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B72" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C72" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B74" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C74" s="21" t="s">
         <v>167</v>
-      </c>
-      <c r="C74" s="21" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="B75" s="21" t="s">
         <v>317</v>
       </c>
-      <c r="B75" s="21" t="s">
-        <v>318</v>
-      </c>
       <c r="C75" s="21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" s="19" t="s">
         <v>142</v>
-      </c>
-      <c r="B78" s="19" t="s">
-        <v>143</v>
       </c>
       <c r="C78" s="19"/>
     </row>
     <row r="79" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B79" s="19" t="s">
         <v>144</v>
-      </c>
-      <c r="B79" s="19" t="s">
-        <v>145</v>
       </c>
       <c r="C79" s="19"/>
     </row>
     <row r="80" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="B80" s="19" t="s">
         <v>253</v>
-      </c>
-      <c r="B80" s="19" t="s">
-        <v>254</v>
       </c>
       <c r="C80" s="19"/>
     </row>
@@ -5093,96 +5173,96 @@
     <row r="82" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="B83" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="B83" s="44" t="s">
-        <v>192</v>
-      </c>
       <c r="C83" s="44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="19"/>
       <c r="B84" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B85" s="19"/>
       <c r="C85" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="86" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B86" s="19"/>
       <c r="C86" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B87" s="19"/>
       <c r="C87" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B88" s="19"/>
       <c r="C88" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="89" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B89" s="19"/>
       <c r="C89" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B90" s="19"/>
       <c r="C90" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="92" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="37" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B92" s="38"/>
       <c r="C92" s="38"/>
     </row>
     <row r="93" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="38" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B93" s="38"/>
       <c r="C93" s="38"/>
     </row>
     <row r="94" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="41" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B94" s="41"/>
       <c r="C94" s="41"/>
@@ -5246,17 +5326,17 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
@@ -5273,7 +5353,7 @@
     </row>
     <row r="5" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B5" s="40"/>
       <c r="C5" s="40"/>
@@ -5290,7 +5370,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
@@ -5307,7 +5387,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -5324,7 +5404,7 @@
     </row>
     <row r="8" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="37"/>
@@ -5341,7 +5421,7 @@
     </row>
     <row r="9" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
@@ -5358,7 +5438,7 @@
     </row>
     <row r="10" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B10" s="37"/>
       <c r="C10" s="37"/>
@@ -5375,7 +5455,7 @@
     </row>
     <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
@@ -5392,7 +5472,7 @@
     </row>
     <row r="12" spans="1:13" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B12" s="37"/>
       <c r="C12" s="37"/>
@@ -5424,7 +5504,7 @@
     </row>
     <row r="14" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" s="40"/>
@@ -5440,13 +5520,13 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="43"/>
       <c r="E15" s="43"/>
@@ -5460,13 +5540,13 @@
     </row>
     <row r="16" spans="1:13" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="C16" s="28" t="s">
         <v>210</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -5476,46 +5556,46 @@
     </row>
     <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B18" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="B19" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="C19" s="20" t="s">
         <v>219</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="C20" s="20" t="s">
         <v>221</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C21" s="29" t="s">
         <v>213</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>212</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -5525,89 +5605,89 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B23" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" s="20" t="s">
         <v>187</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B24" s="46"/>
       <c r="C24" s="46"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B26" s="20"/>
       <c r="C26" s="20"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="20"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B28" s="46"/>
       <c r="C28" s="46"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="46" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B29" s="46"/>
       <c r="C29" s="46"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B30" s="20"/>
       <c r="C30" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B31" s="20"/>
       <c r="C31" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="46" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B32" s="46"/>
       <c r="C32" s="46"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B33" s="20"/>
       <c r="C33" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -5617,248 +5697,248 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="47" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B35" s="47"/>
       <c r="C35" s="47"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C37" s="20"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C38" s="20"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B39" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="C39" s="20" t="s">
         <v>289</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="21" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C40" s="20"/>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C41" s="20"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B44" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="C44" s="19" t="s">
         <v>284</v>
-      </c>
-      <c r="C44" s="19" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C46" s="20"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C47" s="20"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="B48" s="20" t="s">
         <v>305</v>
-      </c>
-      <c r="B48" s="20" t="s">
-        <v>306</v>
       </c>
       <c r="C48" s="20"/>
     </row>
     <row r="49" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="B51" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="C51" s="21" t="s">
         <v>226</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C52" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="48" t="s">
+        <v>277</v>
+      </c>
+      <c r="B53" s="20" t="s">
         <v>278</v>
-      </c>
-      <c r="B53" s="20" t="s">
-        <v>279</v>
       </c>
       <c r="C53" s="20"/>
     </row>
     <row r="54" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B54" s="20" t="s">
         <v>144</v>
-      </c>
-      <c r="B54" s="20" t="s">
-        <v>145</v>
       </c>
       <c r="C54" s="20"/>
     </row>
     <row r="55" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="B55" s="20" t="s">
         <v>253</v>
-      </c>
-      <c r="B55" s="20" t="s">
-        <v>254</v>
       </c>
       <c r="C55" s="20"/>
     </row>
     <row r="56" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="29" t="s">
+        <v>259</v>
+      </c>
+      <c r="B56" s="29" t="s">
         <v>260</v>
-      </c>
-      <c r="B56" s="29" t="s">
-        <v>261</v>
       </c>
       <c r="C56" s="29"/>
     </row>
     <row r="57" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="B58" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="B58" s="44" t="s">
-        <v>192</v>
-      </c>
       <c r="C58" s="44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="19"/>
       <c r="B59" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B60" s="19"/>
       <c r="C60" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D60" s="43"/>
       <c r="E60" s="43"/>
@@ -5873,81 +5953,81 @@
     </row>
     <row r="61" spans="1:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B61" s="19"/>
       <c r="C61" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B62" s="19"/>
       <c r="C62" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B63" s="19"/>
       <c r="C63" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A64" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="B64" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="B64" s="22" t="s">
-        <v>238</v>
-      </c>
       <c r="C64" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A65" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B66" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="C66" s="27" t="s">
         <v>240</v>
-      </c>
-      <c r="C66" s="27" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B68" s="29"/>
       <c r="C68" s="29"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B69" s="38"/>
       <c r="C69" s="38"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="42" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B70" s="42"/>
       <c r="C70" s="42"/>

</xml_diff>